<commit_message>
Folder + files .ipynb
</commit_message>
<xml_diff>
--- a/Income/data/PPI.xlsx
+++ b/Income/data/PPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\GitHub\Python\Projetcs\P3\Data-Manipulation-with-Python\Income\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC4B3C0-C0D0-4A7D-B76A-06A3292F4E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3062803B-FFEA-4CF9-AD8D-575E864D6392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29745" yWindow="-120" windowWidth="27975" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2592,7 +2592,7 @@
   <dimension ref="A1:N2147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2148" sqref="A2148"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>